<commit_message>
P4 hasta Ej 16
</commit_message>
<xml_diff>
--- a/Clase 4/Ejercicio5.xlsx
+++ b/Clase 4/Ejercicio5.xlsx
@@ -119,7 +119,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,12 +128,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -141,17 +147,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -456,1762 +480,2651 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AY41" sqref="AY41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="AQ37" sqref="AQ37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2">
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5">
         <v>0</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="4">
         <v>1</v>
       </c>
-      <c r="F1">
-        <v>2</v>
-      </c>
-      <c r="G1">
-        <v>3</v>
-      </c>
-      <c r="H1">
-        <v>4</v>
-      </c>
-      <c r="I1">
+      <c r="F1" s="4">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4">
         <v>5</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="4">
         <v>6</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="4">
         <v>7</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="4">
         <v>8</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="4">
         <v>9</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="4">
         <v>10</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="4">
         <v>11</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="4">
         <v>12</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="4">
         <v>13</v>
       </c>
-      <c r="R1">
+      <c r="R1" s="4">
         <v>14</v>
       </c>
-      <c r="S1">
+      <c r="S1" s="4">
         <v>15</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="4">
         <v>16</v>
       </c>
-      <c r="U1">
+      <c r="U1" s="4">
         <v>17</v>
       </c>
-      <c r="V1">
+      <c r="V1" s="4">
         <v>18</v>
       </c>
-      <c r="W1">
+      <c r="W1" s="4">
         <v>19</v>
       </c>
-      <c r="X1">
+      <c r="X1" s="4">
         <v>20</v>
       </c>
-      <c r="Y1">
+      <c r="Y1" s="4">
         <v>21</v>
       </c>
-      <c r="Z1">
+      <c r="Z1" s="4">
         <v>22</v>
       </c>
-      <c r="AA1">
+      <c r="AA1" s="4">
         <v>23</v>
       </c>
-      <c r="AB1">
+      <c r="AB1" s="4">
         <v>24</v>
       </c>
-      <c r="AC1">
+      <c r="AC1" s="4">
         <v>25</v>
       </c>
-      <c r="AD1">
+      <c r="AD1" s="4">
         <v>26</v>
       </c>
-      <c r="AE1">
+      <c r="AE1" s="4">
         <v>27</v>
       </c>
-      <c r="AF1">
+      <c r="AF1" s="4">
         <v>28</v>
       </c>
-      <c r="AG1">
+      <c r="AG1" s="4">
         <v>29</v>
       </c>
-      <c r="AH1">
+      <c r="AH1" s="4">
         <v>30</v>
       </c>
-      <c r="AI1">
+      <c r="AI1" s="4">
         <v>31</v>
       </c>
-      <c r="AJ1">
+      <c r="AJ1" s="4">
         <v>32</v>
       </c>
-      <c r="AK1">
+      <c r="AK1" s="4">
         <v>33</v>
       </c>
-      <c r="AL1">
+      <c r="AL1" s="4">
         <v>34</v>
       </c>
-      <c r="AM1">
+      <c r="AM1" s="4">
         <v>35</v>
       </c>
-      <c r="AN1">
+      <c r="AN1" s="4">
         <v>36</v>
       </c>
-      <c r="AO1">
+      <c r="AO1" s="4">
         <v>37</v>
       </c>
-      <c r="AP1">
+      <c r="AP1" s="4">
         <v>38</v>
       </c>
-      <c r="AQ1">
+      <c r="AQ1" s="4">
         <v>39</v>
       </c>
-      <c r="AR1">
+      <c r="AR1" s="4">
         <v>40</v>
       </c>
-      <c r="AS1">
+      <c r="AS1" s="4">
         <v>41</v>
       </c>
-      <c r="AT1">
+      <c r="AT1" s="4">
         <v>42</v>
       </c>
-      <c r="AU1">
+      <c r="AU1" s="4">
         <v>43</v>
       </c>
-      <c r="AV1">
+      <c r="AV1" s="4">
         <v>44</v>
       </c>
-      <c r="AW1">
+      <c r="AW1" s="4">
         <v>45</v>
       </c>
-      <c r="AX1">
+      <c r="AX1" s="4">
         <v>46</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="AY1" s="4"/>
+      <c r="AZ1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BA1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
         <v>5</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AZ2">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1">
         <v>7</v>
       </c>
-      <c r="BA2">
+      <c r="BA2" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>15</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K3">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1">
         <v>1</v>
       </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="M3">
-        <v>3</v>
-      </c>
-      <c r="N3">
-        <v>4</v>
-      </c>
-      <c r="O3">
+      <c r="L3" s="1">
+        <v>2</v>
+      </c>
+      <c r="M3" s="1">
+        <v>3</v>
+      </c>
+      <c r="N3" s="1">
+        <v>4</v>
+      </c>
+      <c r="O3" s="1">
         <v>5</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="1">
         <v>6</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="1">
         <v>7</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="1">
         <v>8</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="1">
         <v>9</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="1">
         <v>10</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="1">
         <v>11</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="1">
         <v>12</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="1">
         <v>13</v>
       </c>
-      <c r="X3">
+      <c r="X3" s="1">
         <v>14</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Y3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AZ3">
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
+      <c r="AW3" s="1"/>
+      <c r="AX3" s="1"/>
+      <c r="AY3" s="1"/>
+      <c r="AZ3" s="1">
         <v>22</v>
       </c>
-      <c r="BA3">
+      <c r="BA3" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Z4">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1">
         <v>1</v>
       </c>
-      <c r="AA4">
-        <v>2</v>
-      </c>
-      <c r="AB4">
-        <v>3</v>
-      </c>
-      <c r="AC4">
-        <v>4</v>
-      </c>
-      <c r="AD4">
+      <c r="AA4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="1">
         <v>5</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="1">
         <v>6</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="1">
         <v>7</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="1">
         <v>8</v>
       </c>
-      <c r="AH4">
+      <c r="AH4" s="1">
         <v>9</v>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="1">
         <v>10</v>
       </c>
-      <c r="AJ4">
+      <c r="AJ4" s="1">
         <v>11</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AK4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AZ4">
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="1"/>
+      <c r="AT4" s="1"/>
+      <c r="AU4" s="1"/>
+      <c r="AV4" s="1"/>
+      <c r="AW4" s="1"/>
+      <c r="AX4" s="1"/>
+      <c r="AY4" s="1"/>
+      <c r="AZ4" s="1">
         <v>34</v>
       </c>
-      <c r="BA4">
+      <c r="BA4" s="1">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AL5">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1">
         <v>1</v>
       </c>
-      <c r="AM5">
-        <v>2</v>
-      </c>
-      <c r="AN5">
-        <v>3</v>
-      </c>
-      <c r="AO5" t="s">
+      <c r="AM5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AN5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AO5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AZ5">
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="1"/>
+      <c r="AT5" s="1"/>
+      <c r="AU5" s="1"/>
+      <c r="AV5" s="1"/>
+      <c r="AW5" s="1"/>
+      <c r="AX5" s="1"/>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1">
         <v>38</v>
       </c>
-      <c r="BA5">
+      <c r="BA5" s="1">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>9</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AP6">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1">
         <v>1</v>
       </c>
-      <c r="AQ6">
-        <v>2</v>
-      </c>
-      <c r="AR6">
-        <v>3</v>
-      </c>
-      <c r="AS6">
-        <v>4</v>
-      </c>
-      <c r="AT6">
+      <c r="AQ6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AR6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AS6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AT6" s="1">
         <v>5</v>
       </c>
-      <c r="AU6">
+      <c r="AU6" s="1">
         <v>6</v>
       </c>
-      <c r="AV6">
+      <c r="AV6" s="1">
         <v>7</v>
       </c>
-      <c r="AW6">
+      <c r="AW6" s="1">
         <v>8</v>
       </c>
-      <c r="AX6" t="s">
+      <c r="AX6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AZ6">
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1">
         <v>47</v>
       </c>
-      <c r="BA6">
+      <c r="BA6" s="1">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="1"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+      <c r="AQ7" s="1"/>
+      <c r="AR7" s="1"/>
+      <c r="AS7" s="1"/>
+      <c r="AT7" s="1"/>
+      <c r="AU7" s="1"/>
+      <c r="AV7" s="1"/>
+      <c r="AW7" s="1"/>
+      <c r="AX7" s="1"/>
+      <c r="AY7" s="1"/>
+      <c r="AZ7" s="1"/>
+      <c r="BA7" s="1"/>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5">
         <v>0</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <v>1</v>
       </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="G13">
-        <v>3</v>
-      </c>
-      <c r="H13">
-        <v>4</v>
-      </c>
-      <c r="I13">
+      <c r="F13" s="4">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4">
+        <v>3</v>
+      </c>
+      <c r="H13" s="4">
+        <v>4</v>
+      </c>
+      <c r="I13" s="4">
         <v>5</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="4">
         <v>6</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="4">
         <v>7</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="4">
         <v>8</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="4">
         <v>9</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="4">
         <v>10</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="4">
         <v>11</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="4">
         <v>12</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="4">
         <v>13</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="4">
         <v>14</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="4">
         <v>15</v>
       </c>
-      <c r="T13">
+      <c r="T13" s="4">
         <v>16</v>
       </c>
-      <c r="U13">
+      <c r="U13" s="4">
         <v>17</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="4">
         <v>18</v>
       </c>
-      <c r="W13">
+      <c r="W13" s="4">
         <v>19</v>
       </c>
-      <c r="X13">
+      <c r="X13" s="4">
         <v>20</v>
       </c>
-      <c r="Y13">
+      <c r="Y13" s="4">
         <v>21</v>
       </c>
-      <c r="Z13">
+      <c r="Z13" s="4">
         <v>22</v>
       </c>
-      <c r="AA13">
+      <c r="AA13" s="4">
         <v>23</v>
       </c>
-      <c r="AB13">
+      <c r="AB13" s="4">
         <v>24</v>
       </c>
-      <c r="AC13">
+      <c r="AC13" s="4">
         <v>25</v>
       </c>
-      <c r="AD13">
+      <c r="AD13" s="4">
         <v>26</v>
       </c>
-      <c r="AE13">
+      <c r="AE13" s="4">
         <v>27</v>
       </c>
-      <c r="AF13">
+      <c r="AF13" s="4">
         <v>28</v>
       </c>
-      <c r="AG13">
+      <c r="AG13" s="4">
         <v>29</v>
       </c>
-      <c r="AH13">
+      <c r="AH13" s="4">
         <v>30</v>
       </c>
-      <c r="AI13">
+      <c r="AI13" s="4">
         <v>31</v>
       </c>
-      <c r="AJ13">
+      <c r="AJ13" s="4">
         <v>32</v>
       </c>
-      <c r="AK13">
+      <c r="AK13" s="4">
         <v>33</v>
       </c>
-      <c r="AL13">
+      <c r="AL13" s="4">
         <v>34</v>
       </c>
-      <c r="AM13">
+      <c r="AM13" s="4">
         <v>35</v>
       </c>
-      <c r="AN13">
+      <c r="AN13" s="4">
         <v>36</v>
       </c>
-      <c r="AO13">
+      <c r="AO13" s="4">
         <v>37</v>
       </c>
-      <c r="AP13">
+      <c r="AP13" s="4">
         <v>38</v>
       </c>
-      <c r="AQ13">
+      <c r="AQ13" s="4">
         <v>39</v>
       </c>
-      <c r="AR13">
+      <c r="AR13" s="4">
         <v>40</v>
       </c>
-      <c r="AS13">
+      <c r="AS13" s="4">
         <v>41</v>
       </c>
-      <c r="AT13">
+      <c r="AT13" s="4">
         <v>42</v>
       </c>
-      <c r="AU13">
+      <c r="AU13" s="4">
         <v>43</v>
       </c>
-      <c r="AV13">
+      <c r="AV13" s="4">
         <v>44</v>
       </c>
-      <c r="AW13">
+      <c r="AW13" s="4">
         <v>45</v>
       </c>
-      <c r="AX13">
+      <c r="AX13" s="4">
         <v>46</v>
       </c>
-      <c r="AZ13" t="s">
+      <c r="AY13" s="4"/>
+      <c r="AZ13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BA13" t="s">
+      <c r="BA13" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
         <v>0</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>7</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H14">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1">
         <v>1</v>
       </c>
-      <c r="I14">
-        <v>2</v>
-      </c>
-      <c r="J14">
-        <v>3</v>
-      </c>
-      <c r="K14">
-        <v>4</v>
-      </c>
-      <c r="L14">
+      <c r="I14" s="1">
+        <v>2</v>
+      </c>
+      <c r="J14" s="1">
+        <v>3</v>
+      </c>
+      <c r="K14" s="1">
+        <v>4</v>
+      </c>
+      <c r="L14" s="1">
         <v>5</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="1">
         <v>6</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AZ14">
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
+      <c r="AR14" s="1"/>
+      <c r="AS14" s="1"/>
+      <c r="AT14" s="1"/>
+      <c r="AU14" s="1"/>
+      <c r="AV14" s="1"/>
+      <c r="AW14" s="1"/>
+      <c r="AX14" s="1"/>
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="1">
         <v>11</v>
       </c>
-      <c r="BA14">
+      <c r="BA14" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
         <v>0</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>15</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AJ15">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1">
         <v>1</v>
       </c>
-      <c r="AK15">
-        <v>2</v>
-      </c>
-      <c r="AL15">
-        <v>3</v>
-      </c>
-      <c r="AM15">
-        <v>4</v>
-      </c>
-      <c r="AN15">
+      <c r="AK15" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AM15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AN15" s="1">
         <v>5</v>
       </c>
-      <c r="AO15">
+      <c r="AO15" s="1">
         <v>6</v>
       </c>
-      <c r="AP15">
+      <c r="AP15" s="1">
         <v>7</v>
       </c>
-      <c r="AQ15">
+      <c r="AQ15" s="1">
         <v>8</v>
       </c>
-      <c r="AR15">
+      <c r="AR15" s="1">
         <v>9</v>
       </c>
-      <c r="AS15">
+      <c r="AS15" s="1">
         <v>10</v>
       </c>
-      <c r="AT15">
+      <c r="AT15" s="1">
         <v>11</v>
       </c>
-      <c r="AU15">
+      <c r="AU15" s="1">
         <v>12</v>
       </c>
-      <c r="AV15">
+      <c r="AV15" s="1">
         <v>13</v>
       </c>
-      <c r="AW15">
+      <c r="AW15" s="1">
         <v>14</v>
       </c>
-      <c r="AX15" t="s">
+      <c r="AX15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AZ15">
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1">
         <v>47</v>
       </c>
-      <c r="BA15">
+      <c r="BA15" s="1">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>0</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>12</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="X16">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1">
         <v>1</v>
       </c>
-      <c r="Y16">
-        <v>2</v>
-      </c>
-      <c r="Z16">
-        <v>3</v>
-      </c>
-      <c r="AA16">
-        <v>4</v>
-      </c>
-      <c r="AB16">
+      <c r="Y16" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB16" s="1">
         <v>5</v>
       </c>
-      <c r="AC16">
+      <c r="AC16" s="1">
         <v>6</v>
       </c>
-      <c r="AD16">
+      <c r="AD16" s="1">
         <v>7</v>
       </c>
-      <c r="AE16">
+      <c r="AE16" s="1">
         <v>8</v>
       </c>
-      <c r="AF16">
+      <c r="AF16" s="1">
         <v>9</v>
       </c>
-      <c r="AG16">
+      <c r="AG16" s="1">
         <v>10</v>
       </c>
-      <c r="AH16">
+      <c r="AH16" s="1">
         <v>11</v>
       </c>
-      <c r="AI16" t="s">
+      <c r="AI16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AZ16">
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="1"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="1"/>
+      <c r="AS16" s="1"/>
+      <c r="AT16" s="1"/>
+      <c r="AU16" s="1"/>
+      <c r="AV16" s="1"/>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="1"/>
+      <c r="AY16" s="1"/>
+      <c r="AZ16" s="1">
         <v>32</v>
       </c>
-      <c r="BA16">
+      <c r="BA16" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>0</v>
       </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>3</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="E17" s="1">
+        <v>2</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AZ17">
-        <v>4</v>
-      </c>
-      <c r="BA17">
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1"/>
+      <c r="AL17" s="1"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="1"/>
+      <c r="AO17" s="1"/>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="1"/>
+      <c r="AS17" s="1"/>
+      <c r="AT17" s="1"/>
+      <c r="AU17" s="1"/>
+      <c r="AV17" s="1"/>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="1"/>
+      <c r="AY17" s="1"/>
+      <c r="AZ17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BA17" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>0</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>9</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O18">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1">
         <v>1</v>
       </c>
-      <c r="P18">
-        <v>2</v>
-      </c>
-      <c r="Q18">
-        <v>3</v>
-      </c>
-      <c r="R18">
-        <v>4</v>
-      </c>
-      <c r="S18">
+      <c r="P18" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>3</v>
+      </c>
+      <c r="R18" s="1">
+        <v>4</v>
+      </c>
+      <c r="S18" s="1">
         <v>5</v>
       </c>
-      <c r="T18">
+      <c r="T18" s="1">
         <v>6</v>
       </c>
-      <c r="U18">
+      <c r="U18" s="1">
         <v>7</v>
       </c>
-      <c r="V18">
+      <c r="V18" s="1">
         <v>8</v>
       </c>
-      <c r="W18" t="s">
+      <c r="W18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AZ18">
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="1"/>
+      <c r="AO18" s="1"/>
+      <c r="AP18" s="1"/>
+      <c r="AQ18" s="1"/>
+      <c r="AR18" s="1"/>
+      <c r="AS18" s="1"/>
+      <c r="AT18" s="1"/>
+      <c r="AU18" s="1"/>
+      <c r="AV18" s="1"/>
+      <c r="AW18" s="1"/>
+      <c r="AX18" s="1"/>
+      <c r="AY18" s="1"/>
+      <c r="AZ18" s="1">
         <v>20</v>
       </c>
-      <c r="BA18">
+      <c r="BA18" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C19" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="1">
-        <v>4</v>
-      </c>
-      <c r="E19" s="1">
+      <c r="D19" s="3">
+        <v>4</v>
+      </c>
+      <c r="E19" s="3">
         <v>1</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="3">
         <v>5</v>
       </c>
-      <c r="G19" s="1">
-        <v>3</v>
-      </c>
-      <c r="H19" s="3">
-        <v>2</v>
-      </c>
-      <c r="AZ19">
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+      <c r="AI19" s="1"/>
+      <c r="AJ19" s="1"/>
+      <c r="AK19" s="1"/>
+      <c r="AL19" s="1"/>
+      <c r="AM19" s="1"/>
+      <c r="AN19" s="1"/>
+      <c r="AO19" s="1"/>
+      <c r="AP19" s="1"/>
+      <c r="AQ19" s="1"/>
+      <c r="AR19" s="1"/>
+      <c r="AS19" s="1"/>
+      <c r="AT19" s="1"/>
+      <c r="AU19" s="1"/>
+      <c r="AV19" s="1"/>
+      <c r="AW19" s="1"/>
+      <c r="AX19" s="1"/>
+      <c r="AY19" s="1"/>
+      <c r="AZ19" s="1">
         <v>22.8</v>
       </c>
-      <c r="BA19">
+      <c r="BA19" s="1">
         <v>13.4</v>
       </c>
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="C24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="5">
         <v>0</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="4">
         <v>1</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="4">
         <v>2</v>
       </c>
       <c r="G24" s="4">
         <v>3</v>
       </c>
-      <c r="H24">
-        <v>4</v>
-      </c>
-      <c r="I24">
+      <c r="H24" s="4">
+        <v>4</v>
+      </c>
+      <c r="I24" s="4">
         <v>5</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="4">
         <v>6</v>
       </c>
       <c r="K24" s="4">
         <v>7</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="4">
         <v>8</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="4">
         <v>9</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="4">
         <v>10</v>
       </c>
       <c r="O24" s="4">
         <v>11</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="4">
         <v>12</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="4">
         <v>13</v>
       </c>
-      <c r="R24">
+      <c r="R24" s="4">
         <v>14</v>
       </c>
       <c r="S24" s="4">
         <v>15</v>
       </c>
-      <c r="T24">
+      <c r="T24" s="4">
         <v>16</v>
       </c>
-      <c r="U24">
+      <c r="U24" s="4">
         <v>17</v>
       </c>
-      <c r="V24">
+      <c r="V24" s="4">
         <v>18</v>
       </c>
       <c r="W24" s="4">
         <v>19</v>
       </c>
-      <c r="X24">
+      <c r="X24" s="4">
         <v>20</v>
       </c>
-      <c r="Y24">
+      <c r="Y24" s="4">
         <v>21</v>
       </c>
-      <c r="Z24">
+      <c r="Z24" s="4">
         <v>22</v>
       </c>
       <c r="AA24" s="4">
         <v>23</v>
       </c>
-      <c r="AB24">
+      <c r="AB24" s="4">
         <v>24</v>
       </c>
-      <c r="AC24">
+      <c r="AC24" s="4">
         <v>25</v>
       </c>
-      <c r="AD24">
+      <c r="AD24" s="4">
         <v>26</v>
       </c>
       <c r="AE24" s="4">
         <v>27</v>
       </c>
-      <c r="AF24">
+      <c r="AF24" s="4">
         <v>28</v>
       </c>
-      <c r="AG24">
+      <c r="AG24" s="4">
         <v>29</v>
       </c>
-      <c r="AH24">
+      <c r="AH24" s="4">
         <v>30</v>
       </c>
       <c r="AI24" s="4">
         <v>31</v>
       </c>
-      <c r="AJ24">
+      <c r="AJ24" s="4">
         <v>32</v>
       </c>
-      <c r="AK24">
+      <c r="AK24" s="4">
         <v>33</v>
       </c>
-      <c r="AL24">
+      <c r="AL24" s="4">
         <v>34</v>
       </c>
       <c r="AM24" s="4">
         <v>35</v>
       </c>
-      <c r="AN24">
+      <c r="AN24" s="4">
         <v>36</v>
       </c>
-      <c r="AO24">
+      <c r="AO24" s="4">
         <v>37</v>
       </c>
-      <c r="AP24">
+      <c r="AP24" s="4">
         <v>38</v>
       </c>
       <c r="AQ24" s="4">
         <v>39</v>
       </c>
-      <c r="AR24">
+      <c r="AR24" s="4">
         <v>40</v>
       </c>
-      <c r="AS24">
+      <c r="AS24" s="4">
         <v>41</v>
       </c>
-      <c r="AT24">
+      <c r="AT24" s="4">
         <v>42</v>
       </c>
       <c r="AU24" s="4">
         <v>43</v>
       </c>
-      <c r="AV24">
+      <c r="AV24" s="4">
         <v>44</v>
       </c>
-      <c r="AW24">
+      <c r="AW24" s="4">
         <v>45</v>
       </c>
-      <c r="AX24">
+      <c r="AX24" s="4">
         <v>46</v>
       </c>
-      <c r="AZ24" t="s">
+      <c r="AY24" s="4"/>
+      <c r="AZ24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BA24" t="s">
+      <c r="BA24" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25">
+      <c r="A25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1">
         <v>0</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>7</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-      <c r="F25">
-        <v>3</v>
-      </c>
-      <c r="G25" s="4">
-        <v>4</v>
-      </c>
-      <c r="K25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25">
+      <c r="E25" s="1">
+        <v>2</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3</v>
+      </c>
+      <c r="G25" s="6">
+        <v>4</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="1">
         <v>5</v>
       </c>
-      <c r="Y25">
+      <c r="Y25" s="1">
         <v>6</v>
       </c>
-      <c r="Z25" t="s">
+      <c r="Z25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA25" s="4"/>
-      <c r="AE25" s="4"/>
-      <c r="AI25" s="4"/>
-      <c r="AM25" s="4"/>
-      <c r="AQ25" s="4"/>
-      <c r="AU25" s="4"/>
-      <c r="AZ25">
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AI25" s="6"/>
+      <c r="AJ25" s="1"/>
+      <c r="AK25" s="1"/>
+      <c r="AL25" s="1"/>
+      <c r="AM25" s="6"/>
+      <c r="AN25" s="1"/>
+      <c r="AO25" s="1"/>
+      <c r="AP25" s="1"/>
+      <c r="AQ25" s="6"/>
+      <c r="AR25" s="1"/>
+      <c r="AS25" s="1"/>
+      <c r="AT25" s="1"/>
+      <c r="AU25" s="6"/>
+      <c r="AV25" s="1"/>
+      <c r="AW25" s="1"/>
+      <c r="AX25" s="1"/>
+      <c r="AY25" s="1"/>
+      <c r="AZ25" s="1">
         <v>23</v>
       </c>
-      <c r="BA25">
+      <c r="BA25" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26">
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1">
         <v>0</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>15</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="H26">
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="1">
         <v>1</v>
       </c>
-      <c r="I26">
-        <v>2</v>
-      </c>
-      <c r="J26">
-        <v>3</v>
-      </c>
-      <c r="K26" s="4">
-        <v>4</v>
-      </c>
-      <c r="O26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="AA26" s="4">
+      <c r="I26" s="1">
+        <v>2</v>
+      </c>
+      <c r="J26" s="1">
+        <v>3</v>
+      </c>
+      <c r="K26" s="6">
+        <v>4</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="6">
         <v>5</v>
       </c>
-      <c r="AE26" s="4"/>
-      <c r="AI26" s="4"/>
-      <c r="AJ26">
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="6"/>
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+      <c r="AI26" s="6"/>
+      <c r="AJ26" s="1">
         <v>6</v>
       </c>
-      <c r="AK26">
+      <c r="AK26" s="1">
         <v>7</v>
       </c>
-      <c r="AL26">
+      <c r="AL26" s="1">
         <v>8</v>
       </c>
-      <c r="AM26" s="4">
+      <c r="AM26" s="6">
         <v>9</v>
       </c>
-      <c r="AQ26" s="4"/>
-      <c r="AS26">
+      <c r="AN26" s="1"/>
+      <c r="AO26" s="1"/>
+      <c r="AP26" s="1"/>
+      <c r="AQ26" s="6"/>
+      <c r="AR26" s="1"/>
+      <c r="AS26" s="1">
         <v>10</v>
       </c>
-      <c r="AT26">
+      <c r="AT26" s="1">
         <v>11</v>
       </c>
-      <c r="AU26" s="4">
+      <c r="AU26" s="6">
         <v>12</v>
       </c>
-      <c r="AV26">
+      <c r="AV26" s="1">
         <v>13</v>
       </c>
-      <c r="AW26">
+      <c r="AW26" s="1">
         <v>14</v>
       </c>
-      <c r="AX26" t="s">
+      <c r="AX26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AZ26">
+      <c r="AY26" s="1"/>
+      <c r="AZ26" s="1">
         <v>47</v>
       </c>
-      <c r="BA26">
+      <c r="BA26" s="1">
         <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>0</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>12</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27">
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="1">
         <v>1</v>
       </c>
-      <c r="M27">
-        <v>2</v>
-      </c>
-      <c r="N27">
-        <v>3</v>
-      </c>
-      <c r="O27" s="4">
-        <v>4</v>
-      </c>
-      <c r="S27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="AA27" s="4"/>
-      <c r="AB27">
+      <c r="M27" s="1">
+        <v>2</v>
+      </c>
+      <c r="N27" s="1">
+        <v>3</v>
+      </c>
+      <c r="O27" s="6">
+        <v>4</v>
+      </c>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="1">
         <v>5</v>
       </c>
-      <c r="AC27">
+      <c r="AC27" s="1">
         <v>6</v>
       </c>
-      <c r="AD27">
+      <c r="AD27" s="1">
         <v>7</v>
       </c>
-      <c r="AE27" s="4">
+      <c r="AE27" s="6">
         <v>8</v>
       </c>
-      <c r="AI27" s="4"/>
-      <c r="AM27" s="4"/>
-      <c r="AN27">
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+      <c r="AI27" s="6"/>
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="1"/>
+      <c r="AL27" s="1"/>
+      <c r="AM27" s="6"/>
+      <c r="AN27" s="1">
         <v>9</v>
       </c>
-      <c r="AO27">
+      <c r="AO27" s="1">
         <v>10</v>
       </c>
-      <c r="AP27">
+      <c r="AP27" s="1">
         <v>11</v>
       </c>
-      <c r="AQ27" s="4" t="s">
+      <c r="AQ27" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AU27" s="4"/>
-      <c r="AZ27">
+      <c r="AR27" s="1"/>
+      <c r="AS27" s="1"/>
+      <c r="AT27" s="1"/>
+      <c r="AU27" s="6"/>
+      <c r="AV27" s="1"/>
+      <c r="AW27" s="1"/>
+      <c r="AX27" s="1"/>
+      <c r="AY27" s="1"/>
+      <c r="AZ27" s="1">
         <v>40</v>
       </c>
-      <c r="BA27">
+      <c r="BA27" s="1">
         <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>0</v>
       </c>
-      <c r="C28">
-        <v>4</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="C28" s="1">
+        <v>4</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28">
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="1">
         <v>1</v>
       </c>
-      <c r="Q28">
-        <v>2</v>
-      </c>
-      <c r="R28">
-        <v>3</v>
-      </c>
-      <c r="S28" s="4" t="s">
+      <c r="Q28" s="1">
+        <v>2</v>
+      </c>
+      <c r="R28" s="1">
+        <v>3</v>
+      </c>
+      <c r="S28" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="W28" s="4"/>
-      <c r="AA28" s="4"/>
-      <c r="AE28" s="4"/>
-      <c r="AI28" s="4"/>
-      <c r="AM28" s="4"/>
-      <c r="AQ28" s="4"/>
-      <c r="AU28" s="4"/>
-      <c r="AZ28">
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="6"/>
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="6"/>
+      <c r="AJ28" s="1"/>
+      <c r="AK28" s="1"/>
+      <c r="AL28" s="1"/>
+      <c r="AM28" s="6"/>
+      <c r="AN28" s="1"/>
+      <c r="AO28" s="1"/>
+      <c r="AP28" s="1"/>
+      <c r="AQ28" s="6"/>
+      <c r="AR28" s="1"/>
+      <c r="AS28" s="1"/>
+      <c r="AT28" s="1"/>
+      <c r="AU28" s="6"/>
+      <c r="AV28" s="1"/>
+      <c r="AW28" s="1"/>
+      <c r="AX28" s="1"/>
+      <c r="AY28" s="1"/>
+      <c r="AZ28" s="1">
         <v>16</v>
       </c>
-      <c r="BA28">
+      <c r="BA28" s="1">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>0</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>9</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29">
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="1">
         <v>1</v>
       </c>
-      <c r="U29">
-        <v>2</v>
-      </c>
-      <c r="V29">
-        <v>3</v>
-      </c>
-      <c r="W29" s="4">
-        <v>4</v>
-      </c>
-      <c r="AA29" s="4"/>
-      <c r="AE29" s="4"/>
-      <c r="AF29">
+      <c r="U29" s="1">
+        <v>2</v>
+      </c>
+      <c r="V29" s="1">
+        <v>3</v>
+      </c>
+      <c r="W29" s="6">
+        <v>4</v>
+      </c>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="6"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="6"/>
+      <c r="AF29" s="1">
         <v>5</v>
       </c>
-      <c r="AG29">
+      <c r="AG29" s="1">
         <v>6</v>
       </c>
-      <c r="AH29">
+      <c r="AH29" s="1">
         <v>7</v>
       </c>
-      <c r="AI29" s="4">
+      <c r="AI29" s="6">
         <v>8</v>
       </c>
-      <c r="AM29" s="4"/>
-      <c r="AQ29" s="4"/>
-      <c r="AR29" t="s">
+      <c r="AJ29" s="1"/>
+      <c r="AK29" s="1"/>
+      <c r="AL29" s="1"/>
+      <c r="AM29" s="6"/>
+      <c r="AN29" s="1"/>
+      <c r="AO29" s="1"/>
+      <c r="AP29" s="1"/>
+      <c r="AQ29" s="6"/>
+      <c r="AR29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AU29" s="4"/>
-      <c r="AZ29">
+      <c r="AS29" s="1"/>
+      <c r="AT29" s="1"/>
+      <c r="AU29" s="6"/>
+      <c r="AV29" s="1"/>
+      <c r="AW29" s="1"/>
+      <c r="AX29" s="1"/>
+      <c r="AY29" s="1"/>
+      <c r="AZ29" s="1">
         <v>41</v>
       </c>
-      <c r="BA29">
+      <c r="BA29" s="1">
         <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="3">
         <v>1</v>
       </c>
-      <c r="E30" s="1">
-        <v>2</v>
-      </c>
-      <c r="F30" s="1">
-        <v>3</v>
-      </c>
-      <c r="G30" s="1">
-        <v>4</v>
-      </c>
-      <c r="H30" s="1">
+      <c r="E30" s="3">
+        <v>2</v>
+      </c>
+      <c r="F30" s="3">
+        <v>3</v>
+      </c>
+      <c r="G30" s="7">
+        <v>4</v>
+      </c>
+      <c r="H30" s="3">
         <v>5</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30" s="3">
         <v>1</v>
       </c>
-      <c r="J30" s="1">
-        <v>2</v>
-      </c>
-      <c r="K30" s="1">
-        <v>3</v>
-      </c>
-      <c r="L30" s="1">
+      <c r="J30" s="3">
+        <v>2</v>
+      </c>
+      <c r="K30" s="7">
+        <v>3</v>
+      </c>
+      <c r="L30" s="3">
         <v>5</v>
       </c>
-      <c r="M30" s="1">
-        <v>2</v>
-      </c>
-      <c r="N30" s="1">
-        <v>3</v>
-      </c>
-      <c r="O30" s="1">
+      <c r="M30" s="3">
+        <v>2</v>
+      </c>
+      <c r="N30" s="3">
+        <v>3</v>
+      </c>
+      <c r="O30" s="7">
         <v>5</v>
       </c>
-      <c r="P30" s="1">
-        <v>2</v>
-      </c>
-      <c r="AZ30">
+      <c r="P30" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="6"/>
+      <c r="AF30" s="1"/>
+      <c r="AG30" s="1"/>
+      <c r="AH30" s="1"/>
+      <c r="AI30" s="6"/>
+      <c r="AJ30" s="1"/>
+      <c r="AK30" s="1"/>
+      <c r="AL30" s="1"/>
+      <c r="AM30" s="6"/>
+      <c r="AN30" s="1"/>
+      <c r="AO30" s="1"/>
+      <c r="AP30" s="1"/>
+      <c r="AQ30" s="6"/>
+      <c r="AR30" s="1"/>
+      <c r="AS30" s="1"/>
+      <c r="AT30" s="1"/>
+      <c r="AU30" s="6"/>
+      <c r="AV30" s="1"/>
+      <c r="AW30" s="1"/>
+      <c r="AX30" s="1"/>
+      <c r="AY30" s="1"/>
+      <c r="AZ30" s="1">
         <v>33.4</v>
       </c>
-      <c r="BA30">
+      <c r="BA30" s="1">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="A36" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="2">
+      <c r="C36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="5">
         <v>0</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="4">
         <v>1</v>
       </c>
-      <c r="F36">
-        <v>2</v>
-      </c>
-      <c r="G36" s="4">
-        <v>3</v>
-      </c>
-      <c r="H36">
-        <v>4</v>
-      </c>
-      <c r="I36">
+      <c r="F36" s="4">
+        <v>2</v>
+      </c>
+      <c r="G36" s="6">
+        <v>3</v>
+      </c>
+      <c r="H36" s="4">
+        <v>4</v>
+      </c>
+      <c r="I36" s="4">
         <v>5</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="4">
         <v>6</v>
       </c>
-      <c r="K36" s="4">
+      <c r="K36" s="6">
         <v>7</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="4">
         <v>8</v>
       </c>
-      <c r="M36">
+      <c r="M36" s="4">
         <v>9</v>
       </c>
-      <c r="N36">
+      <c r="N36" s="4">
         <v>10</v>
       </c>
-      <c r="O36" s="4">
+      <c r="O36" s="6">
         <v>11</v>
       </c>
-      <c r="P36">
+      <c r="P36" s="4">
         <v>12</v>
       </c>
-      <c r="Q36">
+      <c r="Q36" s="4">
         <v>13</v>
       </c>
-      <c r="R36">
+      <c r="R36" s="4">
         <v>14</v>
       </c>
-      <c r="S36" s="4">
+      <c r="S36" s="6">
         <v>15</v>
       </c>
-      <c r="T36">
+      <c r="T36" s="4">
         <v>16</v>
       </c>
-      <c r="U36">
+      <c r="U36" s="4">
         <v>17</v>
       </c>
-      <c r="V36">
+      <c r="V36" s="4">
         <v>18</v>
       </c>
-      <c r="W36" s="4">
+      <c r="W36" s="6">
         <v>19</v>
       </c>
-      <c r="X36">
+      <c r="X36" s="4">
         <v>20</v>
       </c>
-      <c r="Y36">
+      <c r="Y36" s="4">
         <v>21</v>
       </c>
-      <c r="Z36">
+      <c r="Z36" s="4">
         <v>22</v>
       </c>
-      <c r="AA36" s="4">
+      <c r="AA36" s="6">
         <v>23</v>
       </c>
-      <c r="AB36">
+      <c r="AB36" s="4">
         <v>24</v>
       </c>
-      <c r="AC36">
+      <c r="AC36" s="4">
         <v>25</v>
       </c>
-      <c r="AD36">
+      <c r="AD36" s="4">
         <v>26</v>
       </c>
-      <c r="AE36" s="4">
+      <c r="AE36" s="6">
         <v>27</v>
       </c>
-      <c r="AF36">
+      <c r="AF36" s="4">
         <v>28</v>
       </c>
-      <c r="AG36">
+      <c r="AG36" s="4">
         <v>29</v>
       </c>
-      <c r="AH36">
+      <c r="AH36" s="4">
         <v>30</v>
       </c>
-      <c r="AI36" s="4">
+      <c r="AI36" s="6">
         <v>31</v>
       </c>
-      <c r="AJ36">
+      <c r="AJ36" s="4">
         <v>32</v>
       </c>
-      <c r="AK36">
+      <c r="AK36" s="4">
         <v>33</v>
       </c>
-      <c r="AL36">
+      <c r="AL36" s="4">
         <v>34</v>
       </c>
-      <c r="AM36" s="4">
+      <c r="AM36" s="6">
         <v>35</v>
       </c>
-      <c r="AN36">
+      <c r="AN36" s="4">
         <v>36</v>
       </c>
-      <c r="AO36">
+      <c r="AO36" s="4">
         <v>37</v>
       </c>
-      <c r="AP36">
+      <c r="AP36" s="4">
         <v>38</v>
       </c>
-      <c r="AQ36" s="4">
+      <c r="AQ36" s="6">
         <v>39</v>
       </c>
-      <c r="AR36">
+      <c r="AR36" s="4">
         <v>40</v>
       </c>
-      <c r="AS36">
+      <c r="AS36" s="4">
         <v>41</v>
       </c>
-      <c r="AT36">
+      <c r="AT36" s="4">
         <v>42</v>
       </c>
-      <c r="AU36" s="4">
+      <c r="AU36" s="6">
         <v>43</v>
       </c>
-      <c r="AV36">
+      <c r="AV36" s="4">
         <v>44</v>
       </c>
-      <c r="AW36">
+      <c r="AW36" s="4">
         <v>45</v>
       </c>
-      <c r="AX36">
+      <c r="AX36" s="4">
         <v>46</v>
       </c>
-      <c r="AZ36" t="s">
+      <c r="AY36" s="4"/>
+      <c r="AZ36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BA36" t="s">
+      <c r="BA36" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37">
+      <c r="A37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="1">
         <v>0</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>7</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37">
-        <v>3</v>
-      </c>
-      <c r="G37">
-        <v>4</v>
-      </c>
-      <c r="X37">
+      <c r="E37" s="1">
+        <v>2</v>
+      </c>
+      <c r="F37" s="1">
+        <v>3</v>
+      </c>
+      <c r="G37" s="1">
+        <v>4</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1">
         <v>5</v>
       </c>
-      <c r="Y37">
+      <c r="Y37" s="1">
         <v>6</v>
       </c>
-      <c r="Z37" t="s">
+      <c r="Z37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AZ37">
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="1"/>
+      <c r="AC37" s="1"/>
+      <c r="AD37" s="1"/>
+      <c r="AE37" s="1"/>
+      <c r="AF37" s="1"/>
+      <c r="AG37" s="1"/>
+      <c r="AH37" s="1"/>
+      <c r="AI37" s="1"/>
+      <c r="AJ37" s="1"/>
+      <c r="AK37" s="1"/>
+      <c r="AL37" s="1"/>
+      <c r="AM37" s="1"/>
+      <c r="AN37" s="1"/>
+      <c r="AO37" s="1"/>
+      <c r="AP37" s="1"/>
+      <c r="AQ37" s="1"/>
+      <c r="AR37" s="1"/>
+      <c r="AS37" s="1"/>
+      <c r="AT37" s="1"/>
+      <c r="AU37" s="1"/>
+      <c r="AV37" s="1"/>
+      <c r="AW37" s="1"/>
+      <c r="AX37" s="1"/>
+      <c r="AY37" s="1"/>
+      <c r="AZ37" s="1">
         <v>23</v>
       </c>
-      <c r="BA37">
+      <c r="BA37" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38">
+      <c r="A38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1">
         <v>0</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>15</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H38">
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1">
         <v>1</v>
       </c>
-      <c r="I38">
-        <v>2</v>
-      </c>
-      <c r="J38">
-        <v>3</v>
-      </c>
-      <c r="K38">
-        <v>4</v>
-      </c>
-      <c r="AA38">
+      <c r="I38" s="1">
+        <v>2</v>
+      </c>
+      <c r="J38" s="1">
+        <v>3</v>
+      </c>
+      <c r="K38" s="1">
+        <v>4</v>
+      </c>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1">
         <v>5</v>
       </c>
-      <c r="AB38">
+      <c r="AB38" s="1">
         <v>6</v>
       </c>
-      <c r="AC38">
+      <c r="AC38" s="1">
         <v>7</v>
       </c>
-      <c r="AD38">
+      <c r="AD38" s="1">
         <v>8</v>
       </c>
-      <c r="AM38">
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="1"/>
+      <c r="AG38" s="1"/>
+      <c r="AH38" s="1"/>
+      <c r="AI38" s="1"/>
+      <c r="AJ38" s="1"/>
+      <c r="AK38" s="1"/>
+      <c r="AL38" s="1"/>
+      <c r="AM38" s="1">
         <v>9</v>
       </c>
-      <c r="AN38">
+      <c r="AN38" s="1">
         <v>10</v>
       </c>
-      <c r="AO38">
+      <c r="AO38" s="1">
         <v>11</v>
       </c>
-      <c r="AP38">
+      <c r="AP38" s="1">
         <v>12</v>
       </c>
-      <c r="AV38">
+      <c r="AQ38" s="1"/>
+      <c r="AR38" s="1"/>
+      <c r="AS38" s="1"/>
+      <c r="AT38" s="1"/>
+      <c r="AU38" s="1"/>
+      <c r="AV38" s="1">
         <v>13</v>
       </c>
-      <c r="AW38">
+      <c r="AW38" s="1">
         <v>14</v>
       </c>
-      <c r="AX38" t="s">
+      <c r="AX38" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AZ38">
+      <c r="AY38" s="1"/>
+      <c r="AZ38" s="1">
         <v>47</v>
       </c>
-      <c r="BA38">
+      <c r="BA38" s="1">
         <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>0</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>12</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L39">
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1">
         <v>1</v>
       </c>
-      <c r="M39">
-        <v>2</v>
-      </c>
-      <c r="N39">
-        <v>3</v>
-      </c>
-      <c r="O39">
-        <v>4</v>
-      </c>
-      <c r="AE39">
+      <c r="M39" s="1">
+        <v>2</v>
+      </c>
+      <c r="N39" s="1">
+        <v>3</v>
+      </c>
+      <c r="O39" s="1">
+        <v>4</v>
+      </c>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1"/>
+      <c r="AB39" s="1"/>
+      <c r="AC39" s="1"/>
+      <c r="AD39" s="1"/>
+      <c r="AE39" s="1">
         <v>5</v>
       </c>
-      <c r="AF39">
+      <c r="AF39" s="1">
         <v>6</v>
       </c>
-      <c r="AG39">
+      <c r="AG39" s="1">
         <v>7</v>
       </c>
-      <c r="AH39">
+      <c r="AH39" s="1">
         <v>8</v>
       </c>
-      <c r="AQ39">
+      <c r="AI39" s="1"/>
+      <c r="AJ39" s="1"/>
+      <c r="AK39" s="1"/>
+      <c r="AL39" s="1"/>
+      <c r="AM39" s="1"/>
+      <c r="AN39" s="1"/>
+      <c r="AO39" s="1"/>
+      <c r="AP39" s="1"/>
+      <c r="AQ39" s="1">
         <v>9</v>
       </c>
-      <c r="AR39">
+      <c r="AR39" s="1">
         <v>10</v>
       </c>
-      <c r="AS39">
+      <c r="AS39" s="1">
         <v>11</v>
       </c>
-      <c r="AT39" t="s">
+      <c r="AT39" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AZ39">
+      <c r="AU39" s="1"/>
+      <c r="AV39" s="1"/>
+      <c r="AW39" s="1"/>
+      <c r="AX39" s="1"/>
+      <c r="AY39" s="1"/>
+      <c r="AZ39" s="1">
         <v>43</v>
       </c>
-      <c r="BA39">
+      <c r="BA39" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>0</v>
       </c>
-      <c r="C40">
-        <v>4</v>
-      </c>
-      <c r="D40" s="3" t="s">
+      <c r="C40" s="1">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P40">
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1">
         <v>1</v>
       </c>
-      <c r="Q40">
-        <v>2</v>
-      </c>
-      <c r="R40">
-        <v>3</v>
-      </c>
-      <c r="S40" t="s">
+      <c r="Q40" s="1">
+        <v>2</v>
+      </c>
+      <c r="R40" s="1">
+        <v>3</v>
+      </c>
+      <c r="S40" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AZ40">
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1"/>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
+      <c r="AB40" s="1"/>
+      <c r="AC40" s="1"/>
+      <c r="AD40" s="1"/>
+      <c r="AE40" s="1"/>
+      <c r="AF40" s="1"/>
+      <c r="AG40" s="1"/>
+      <c r="AH40" s="1"/>
+      <c r="AI40" s="1"/>
+      <c r="AJ40" s="1"/>
+      <c r="AK40" s="1"/>
+      <c r="AL40" s="1"/>
+      <c r="AM40" s="1"/>
+      <c r="AN40" s="1"/>
+      <c r="AO40" s="1"/>
+      <c r="AP40" s="1"/>
+      <c r="AQ40" s="1"/>
+      <c r="AR40" s="1"/>
+      <c r="AS40" s="1"/>
+      <c r="AT40" s="1"/>
+      <c r="AU40" s="1"/>
+      <c r="AV40" s="1"/>
+      <c r="AW40" s="1"/>
+      <c r="AX40" s="1"/>
+      <c r="AY40" s="1"/>
+      <c r="AZ40" s="1">
         <v>16</v>
       </c>
-      <c r="BA40">
+      <c r="BA40" s="1">
         <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>0</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>9</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="T41">
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1">
         <v>1</v>
       </c>
-      <c r="U41">
-        <v>2</v>
-      </c>
-      <c r="V41">
-        <v>3</v>
-      </c>
-      <c r="W41">
-        <v>4</v>
-      </c>
-      <c r="AI41">
+      <c r="U41" s="1">
+        <v>2</v>
+      </c>
+      <c r="V41" s="1">
+        <v>3</v>
+      </c>
+      <c r="W41" s="1">
+        <v>4</v>
+      </c>
+      <c r="X41" s="1"/>
+      <c r="Y41" s="1"/>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1"/>
+      <c r="AB41" s="1"/>
+      <c r="AC41" s="1"/>
+      <c r="AD41" s="1"/>
+      <c r="AE41" s="1"/>
+      <c r="AF41" s="1"/>
+      <c r="AG41" s="1"/>
+      <c r="AH41" s="1"/>
+      <c r="AI41" s="1">
         <v>5</v>
       </c>
-      <c r="AJ41">
+      <c r="AJ41" s="1">
         <v>6</v>
       </c>
-      <c r="AK41">
+      <c r="AK41" s="1">
         <v>7</v>
       </c>
-      <c r="AL41">
+      <c r="AL41" s="1">
         <v>8</v>
       </c>
-      <c r="AU41" t="s">
+      <c r="AM41" s="1"/>
+      <c r="AN41" s="1"/>
+      <c r="AO41" s="1"/>
+      <c r="AP41" s="1"/>
+      <c r="AQ41" s="1"/>
+      <c r="AR41" s="1"/>
+      <c r="AS41" s="1"/>
+      <c r="AT41" s="1"/>
+      <c r="AU41" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AZ41">
+      <c r="AV41" s="1"/>
+      <c r="AW41" s="1"/>
+      <c r="AX41" s="1"/>
+      <c r="AY41" s="1"/>
+      <c r="AZ41" s="1">
         <v>44</v>
       </c>
-      <c r="BA41">
+      <c r="BA41" s="1">
         <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="3">
         <v>1</v>
       </c>
-      <c r="AZ42">
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+      <c r="Y42" s="1"/>
+      <c r="Z42" s="1"/>
+      <c r="AA42" s="1"/>
+      <c r="AB42" s="1"/>
+      <c r="AC42" s="1"/>
+      <c r="AD42" s="1"/>
+      <c r="AE42" s="1"/>
+      <c r="AF42" s="1"/>
+      <c r="AG42" s="1"/>
+      <c r="AH42" s="1"/>
+      <c r="AI42" s="1"/>
+      <c r="AJ42" s="1"/>
+      <c r="AK42" s="1"/>
+      <c r="AL42" s="1"/>
+      <c r="AM42" s="1"/>
+      <c r="AN42" s="1"/>
+      <c r="AO42" s="1"/>
+      <c r="AP42" s="1"/>
+      <c r="AQ42" s="1"/>
+      <c r="AR42" s="1"/>
+      <c r="AS42" s="1"/>
+      <c r="AT42" s="1"/>
+      <c r="AU42" s="1"/>
+      <c r="AV42" s="1"/>
+      <c r="AW42" s="1"/>
+      <c r="AX42" s="1"/>
+      <c r="AY42" s="1"/>
+      <c r="AZ42" s="1">
         <v>34.6</v>
       </c>
-      <c r="BA42">
+      <c r="BA42" s="1">
         <v>25.2</v>
       </c>
     </row>

</xml_diff>